<commit_message>
Atualização do código do projeto Z005
</commit_message>
<xml_diff>
--- a/dbProjectData_modificado.xlsx
+++ b/dbProjectData_modificado.xlsx
@@ -467,7 +467,7 @@
         <v>31.1342019</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -518,7 +518,7 @@
         <v>-73.985428</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>